<commit_message>
Api working with frontend (proxy). Testing various Material-ui components for card lists and popper images
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D5BA0D57-74A4-4401-81DE-73B888F19737}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C35B8F28-1B3B-48F0-98D1-BE09653741B5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3195" yWindow="3900" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Task</t>
   </si>
@@ -44,9 +44,6 @@
   </si>
   <si>
     <t>Created the repo</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - 16.06.2019</t>
   </si>
   <si>
     <t>Working out how to use SQLAlchemy with Flask and trying to
@@ -68,6 +65,21 @@
   </si>
   <si>
     <t>Also added the full mtg set data to the API is a similar way</t>
+  </si>
+  <si>
+    <t>24.06.2019 - 
+26.06.2019</t>
+  </si>
+  <si>
+    <t>Working out how to connect backend with a 
+minimal frontend app with proxy</t>
+  </si>
+  <si>
+    <t>26.06.2019 - 
+27.06.2019</t>
+  </si>
+  <si>
+    <t>Researching and testing Material-ui styles, tables and poppers and other related components for presenting lists of cards and their respective images</t>
   </si>
 </sst>
 </file>
@@ -432,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,7 +470,7 @@
     </row>
     <row r="2" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
@@ -480,10 +492,10 @@
     </row>
     <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4">
         <v>6</v>
@@ -491,10 +503,10 @@
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5">
         <v>3</v>
@@ -502,13 +514,35 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6">
         <v>1.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Card image popper is now faster and more convenient
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C35B8F28-1B3B-48F0-98D1-BE09653741B5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2892209-CC42-4D56-B77F-EEFB741ABAFF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3195" yWindow="3900" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Task</t>
   </si>
@@ -80,6 +80,13 @@
   </si>
   <si>
     <t>Researching and testing Material-ui styles, tables and poppers and other related components for presenting lists of cards and their respective images</t>
+  </si>
+  <si>
+    <t>28.06.2019</t>
+  </si>
+  <si>
+    <t>Card image Popper now opens up nicely above the card text 
+line when hovering the mouse over it</t>
   </si>
 </sst>
 </file>
@@ -444,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -545,6 +552,17 @@
         <v>6</v>
       </c>
     </row>
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed erros and reseached&tested better ways of applying Material-ui styles to custom components
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2892209-CC42-4D56-B77F-EEFB741ABAFF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82FFBB4B-E092-4EC8-A623-0C8D4D03C704}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3195" yWindow="3900" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>Task</t>
   </si>
@@ -87,6 +87,13 @@
   <si>
     <t>Card image Popper now opens up nicely above the card text 
 line when hovering the mouse over it</t>
+  </si>
+  <si>
+    <t>Fixed erros and reseached&amp;tested better ways of applying Material-ui styles to custom components</t>
+  </si>
+  <si>
+    <t>01.07.2019 - 
+04.07.2019</t>
   </si>
 </sst>
 </file>
@@ -451,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,6 +570,17 @@
         <v>3</v>
       </c>
     </row>
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Added fonts for displaying various Mtg symbols such as manacosts and card types
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82FFBB4B-E092-4EC8-A623-0C8D4D03C704}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10C634FD-3358-4C39-8624-F55ABBA4C930}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>Task</t>
   </si>
@@ -94,6 +94,13 @@
   <si>
     <t>01.07.2019 - 
 04.07.2019</t>
+  </si>
+  <si>
+    <t>04.07.2019</t>
+  </si>
+  <si>
+    <t>Added fonts for displaying various Mtg symbols such as
+manacosts and card types</t>
   </si>
 </sst>
 </file>
@@ -458,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,6 +588,17 @@
         <v>6</v>
       </c>
     </row>
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Added a component to display cards' manacosts
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10C634FD-3358-4C39-8624-F55ABBA4C930}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D740A1F-E5F6-4262-8336-AF72510D443E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Task</t>
   </si>
@@ -101,6 +101,12 @@
   <si>
     <t>Added fonts for displaying various Mtg symbols such as
 manacosts and card types</t>
+  </si>
+  <si>
+    <t>05.07.2019</t>
+  </si>
+  <si>
+    <t>Added a component to correctly display cards' manacosts</t>
   </si>
 </sst>
 </file>
@@ -465,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,6 +605,17 @@
         <v>1</v>
       </c>
     </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
The Card objects from the api are now returned  paginated
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D740A1F-E5F6-4262-8336-AF72510D443E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{513BAE04-5DD2-4DB1-BB69-E22B455C17E5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21480" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>Task</t>
   </si>
@@ -107,6 +107,13 @@
   </si>
   <si>
     <t>Added a component to correctly display cards' manacosts</t>
+  </si>
+  <si>
+    <t>08.07.2019</t>
+  </si>
+  <si>
+    <t>The Card objects from the api are now returned 
+paginated with additional info such as the link for the next page and the total number of cards and pages. This is because the json for all the cards is too big and slow.</t>
   </si>
 </sst>
 </file>
@@ -471,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,6 +623,17 @@
         <v>2</v>
       </c>
     </row>
+    <row r="13" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13">
+        <v>1.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Added colos as a seperate table for applying filters. Testing reading url parameters and query strings
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF633405-5AAB-4476-9498-57A2C20463B4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3B72CB4-72E4-4F38-8403-0CD2BC8C75FE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="390" windowWidth="21480" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>Task</t>
   </si>
@@ -114,6 +114,13 @@
   <si>
     <t>The Card objects from the api are now returned 
 paginated with additional info such as the link for the next page and the total number of cards and pages. This is because the json for all the cards is too big and slow.</t>
+  </si>
+  <si>
+    <t>09.07.2019 - 
+11.07.2019</t>
+  </si>
+  <si>
+    <t>Researching on handling url parameters and query strings with get requests. Researching on how to do a bit more complex searches with SQLAlchemy. Working towards better queries and more robust database without PickleTypes which can't be used for filtering. Added the cards' colors as a separate table which can now be used as a filter.</t>
   </si>
 </sst>
 </file>
@@ -478,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,6 +641,17 @@
         <v>1.5</v>
       </c>
     </row>
+    <row r="14" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Added a route to get a booster pack-like random sample from a set. Various arguments can be specified such as the number of commons, uncommons rares etc.
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3B72CB4-72E4-4F38-8403-0CD2BC8C75FE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA14307C-2A47-4D8A-8FDD-6437D9F23E84}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21480" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
   <si>
     <t>Task</t>
   </si>
@@ -121,6 +121,13 @@
   </si>
   <si>
     <t>Researching on handling url parameters and query strings with get requests. Researching on how to do a bit more complex searches with SQLAlchemy. Working towards better queries and more robust database without PickleTypes which can't be used for filtering. Added the cards' colors as a separate table which can now be used as a filter.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+15.07.2019</t>
+  </si>
+  <si>
+    <t>The backend has now a route for generating booster pack-like random samples from sets. It accepts arguments for the number of commons, uncommons and rares to add to the pack as well as if a basic land is to be added</t>
   </si>
 </sst>
 </file>
@@ -207,7 +214,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normaali" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -485,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -652,6 +659,17 @@
         <v>12</v>
       </c>
     </row>
+    <row r="15" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15">
+        <v>4.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Added a footer. Added a lazy-loading imagelist for viewing lists of cards as a grid of card images with rounded borders.
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA14307C-2A47-4D8A-8FDD-6437D9F23E84}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7AB8D2F-C192-4DCE-9B57-F26A9F968ADC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>Task</t>
   </si>
@@ -128,6 +128,13 @@
   </si>
   <si>
     <t>The backend has now a route for generating booster pack-like random samples from sets. It accepts arguments for the number of commons, uncommons and rares to add to the pack as well as if a basic land is to be added</t>
+  </si>
+  <si>
+    <t>16.07.2019 - 
+18.07.2019</t>
+  </si>
+  <si>
+    <t>Added a footer for the site. Fiddled around with css elements on various similar sites and tested how to do better page layouts. Added lazy-loading imagelist for viewing lists of cards as just a grid of card images with rounded borders.</t>
   </si>
 </sst>
 </file>
@@ -492,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -670,6 +677,17 @@
         <v>4.5</v>
       </c>
     </row>
+    <row r="16" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Double-sided cards can now be flipped over to show their backsides
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7AB8D2F-C192-4DCE-9B57-F26A9F968ADC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A743B8B5-D4AB-41E0-B034-857BA1CA98C4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="840" windowWidth="21600" windowHeight="14145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>Task</t>
   </si>
@@ -135,6 +135,13 @@
   </si>
   <si>
     <t>Added a footer for the site. Fiddled around with css elements on various similar sites and tested how to do better page layouts. Added lazy-loading imagelist for viewing lists of cards as just a grid of card images with rounded borders.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 
+18.07.2019</t>
+  </si>
+  <si>
+    <t>Refractored the code a bit. Added a hidden button on the card images to flip them over in case they are double-sided. The button is visible only when mouse enters a card which is double-sided. Clicking the button switches to the backside</t>
   </si>
 </sst>
 </file>
@@ -499,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -688,6 +695,17 @@
         <v>10</v>
       </c>
     </row>
+    <row r="17" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Small refractors. Added Routes in the backend for set codes. Added some components and Stories for a single card info View. Added the Roboto font and small base theme to apply across the app.
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A743B8B5-D4AB-41E0-B034-857BA1CA98C4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46C494BE-E150-4C10-8A6D-D1AD52293033}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="840" windowWidth="21600" windowHeight="14145" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="840" windowWidth="21600" windowHeight="14460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t>Task</t>
   </si>
@@ -142,16 +142,27 @@
   </si>
   <si>
     <t>Refractored the code a bit. Added a hidden button on the card images to flip them over in case they are double-sided. The button is visible only when mouse enters a card which is double-sided. Clicking the button switches to the backside</t>
+  </si>
+  <si>
+    <t>Changed the routes for sets by the set code instead of id. The codes are unique and easier to read. Also added a quick route to get the cards of a set. Added the corresponding services for react.</t>
+  </si>
+  <si>
+    <t>Checking out Storybook for viewing&amp;styling single components. No need to render the full app too see a component.</t>
+  </si>
+  <si>
+    <t>Worked out how to load custom fonts for Storybook. 
+Installed the Google Roboto font and added a tiny theme to apply the font through. Working towards a View for the info of a single card, added a few components and Stories for this view.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="d\.m\.yy;@"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -167,13 +178,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -183,7 +187,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -206,26 +210,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normaali" xfId="0" builtinId="0"/>
@@ -506,24 +535,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.140625" customWidth="1"/>
-    <col min="2" max="2" width="56.140625" customWidth="1"/>
-    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="56.140625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="10" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="4" t="s">
@@ -531,183 +560,222 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="5">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="5">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="5">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="5">
         <v>1.5</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="5">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="5">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="5">
         <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="5">
         <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="5">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="5">
         <v>1.5</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+    <row r="14" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="5">
         <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="5">
         <v>4.5</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="5">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+    <row r="17" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="5">
         <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>43664</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>43669</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="5">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>43669</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1048576" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C1048576" s="6">
+        <f>COUNT(C2:C1048575)</f>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Card info box ready. Refractors.
Card info box showing all the main card stats such as the name, power/toughness, type, legalities etc. is now done. It takes into account if the card has multiple faces. Refractored the code a bit again, moved components under another folder for better filestructure.
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46C494BE-E150-4C10-8A6D-D1AD52293033}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A971A99-0830-40C0-9B21-0C24E6A5986D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="840" windowWidth="21600" windowHeight="14460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t>Task</t>
   </si>
@@ -152,6 +152,9 @@
   <si>
     <t>Worked out how to load custom fonts for Storybook. 
 Installed the Google Roboto font and added a tiny theme to apply the font through. Working towards a View for the info of a single card, added a few components and Stories for this view.</t>
+  </si>
+  <si>
+    <t>Card info box showing all the main card stats such as the name, power/toughness, type, legalities etc. is now done. It takes into account if the card has multiple faces. Refractored the code a bit again, moved components under another folder for better filestructure.</t>
   </si>
 </sst>
 </file>
@@ -537,8 +540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -768,10 +771,21 @@
         <v>5</v>
       </c>
     </row>
+    <row r="21" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>43670</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="6">
+        <v>5</v>
+      </c>
+    </row>
     <row r="1048576" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1048576" s="6">
         <f>COUNT(C2:C1048575)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed flipbutton placement and it can now also flip card images upside down
The flip button on top of card images can now also flip the
cards upside-down if the card's layout is flippable. The button is also now always on the correct position no matter how big the card image is.
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A971A99-0830-40C0-9B21-0C24E6A5986D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4668333-0736-438B-9B9F-A1183A7FC144}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="840" windowWidth="21600" windowHeight="14460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>Task</t>
   </si>
@@ -155,6 +155,10 @@
   </si>
   <si>
     <t>Card info box showing all the main card stats such as the name, power/toughness, type, legalities etc. is now done. It takes into account if the card has multiple faces. Refractored the code a bit again, moved components under another folder for better filestructure.</t>
+  </si>
+  <si>
+    <t>The flip button on top of card images can now also flip the 
+cards upside-down if the card's layout is flippable. The button is also now always on the correct position no matter how big the card image is.</t>
   </si>
 </sst>
 </file>
@@ -541,7 +545,7 @@
   <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -782,10 +786,21 @@
         <v>5</v>
       </c>
     </row>
+    <row r="22" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>43670</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="6">
+        <v>1.5</v>
+      </c>
+    </row>
     <row r="1048576" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1048576" s="6">
         <f>COUNT(C2:C1048575)</f>
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refractoring the folder structure. Card images are now lazyloading with card-back placeholders.
Refractored the component folder structure. The card images now lazyload by default having a correct-sized card-back image as a placeholder.
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4668333-0736-438B-9B9F-A1183A7FC144}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE137536-193D-48F5-82D6-911142F73489}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="840" windowWidth="21600" windowHeight="14460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
   <si>
     <t>Task</t>
   </si>
@@ -159,6 +159,10 @@
   <si>
     <t>The flip button on top of card images can now also flip the 
 cards upside-down if the card's layout is flippable. The button is also now always on the correct position no matter how big the card image is.</t>
+  </si>
+  <si>
+    <t>The card images now lazyload by default having a 
+correct-sized card-back image as a placeholder.</t>
   </si>
 </sst>
 </file>
@@ -545,7 +549,7 @@
   <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -797,10 +801,21 @@
         <v>1.5</v>
       </c>
     </row>
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>43671</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C23" s="6">
+        <v>2.5</v>
+      </c>
+    </row>
     <row r="1048576" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1048576" s="6">
         <f>COUNT(C2:C1048575)</f>
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a basic route to show cards of sets as a grid
Checking out routing for react. Added one basic route to
show a view of the cards of sets as an image grid
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C59F75C4-F18C-4580-A477-5C9F765B830C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B9E989A-3B3A-4C74-8E99-889FBAC04D5C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="840" windowWidth="21600" windowHeight="14460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t>Task</t>
   </si>
@@ -162,6 +162,10 @@
   </si>
   <si>
     <t>Refractored the component folder structure. The card images now lazyload by default having a correct-sized card-back image as a placeholder.</t>
+  </si>
+  <si>
+    <t>Checking out routing for react. Added one basic route to 
+show a view of the cards of sets as an image grid</t>
   </si>
 </sst>
 </file>
@@ -548,7 +552,7 @@
   <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -811,10 +815,21 @@
         <v>2.5</v>
       </c>
     </row>
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>43671</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="6">
+        <v>2</v>
+      </c>
+    </row>
     <row r="1048576" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1048576" s="6">
         <f>COUNT(C2:C1048575)</f>
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Small refractors. Working on a better card table. Figuring out useEffect.
Small refractors. Trying to figure out how to use useEffect. Working on a better card table. Trying to make events related to card tables faster and trying to figure out how to set correct coordinates for popup images
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B9E989A-3B3A-4C74-8E99-889FBAC04D5C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{259901FE-D0FA-460B-9094-2F238AB034AA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="840" windowWidth="21600" windowHeight="14460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
   <si>
     <t>Task</t>
   </si>
@@ -166,6 +166,9 @@
   <si>
     <t>Checking out routing for react. Added one basic route to 
 show a view of the cards of sets as an image grid</t>
+  </si>
+  <si>
+    <t>Small refractors. Working on a better card table. Trying to make events related to card tables faster and trying to figure out how to set correct coordinates for popup images</t>
   </si>
 </sst>
 </file>
@@ -552,7 +555,7 @@
   <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -826,10 +829,21 @@
         <v>2</v>
       </c>
     </row>
+    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>43672</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" s="6">
+        <v>4</v>
+      </c>
+    </row>
     <row r="1048576" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1048576" s="6">
         <f>COUNT(C2:C1048575)</f>
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Styled card tables. Card table image popover works. Card table rows are now links to the card's own view
Styled the card table nicely. The table now shows the card image when hovering the mouse over it and also works as a link to the card's own view. It works ok in a prod build
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{259901FE-D0FA-460B-9094-2F238AB034AA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7BA7186-EC4B-4370-AC7A-55B39B8C1BEE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="840" windowWidth="21600" windowHeight="14460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2865" yWindow="825" windowWidth="21600" windowHeight="14460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
   <si>
     <t>Task</t>
   </si>
@@ -168,7 +168,17 @@
 show a view of the cards of sets as an image grid</t>
   </si>
   <si>
-    <t>Small refractors. Working on a better card table. Trying to make events related to card tables faster and trying to figure out how to set correct coordinates for popup images</t>
+    <t>Small refractors. Trying to figure out how to use useEffect. Working on a better card table. Trying to make events related to card tables faster and trying to figure out how to set correct coordinates for popup images</t>
+  </si>
+  <si>
+    <t>27/07/2019 - 
+29/07/2019</t>
+  </si>
+  <si>
+    <t>Debugging a problem with a very slow mouseMove-eventhandler attached to a window containing a table. For some reason it fires hundreds of invokeGuardedCallback-events. Concluded it should go away in a production build</t>
+  </si>
+  <si>
+    <t>Styled the card table nicely. The table now shows the card image when hovering the mouse over it and also works as a link to the card's own view</t>
   </si>
 </sst>
 </file>
@@ -244,7 +254,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -272,6 +282,9 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="4"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normaali" xfId="0" builtinId="0"/>
@@ -554,8 +567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -829,7 +842,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>43672</v>
       </c>
@@ -839,11 +852,171 @@
       <c r="C25" s="6">
         <v>4</v>
       </c>
+    </row>
+    <row r="26" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A26" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>43675</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="8"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="8"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="8"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="8"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B32" s="8"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="8"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="8"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="8"/>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="8"/>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" s="8"/>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B38" s="8"/>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B39" s="8"/>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B40" s="8"/>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B41" s="8"/>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B42" s="8"/>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B43" s="8"/>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B44" s="8"/>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B45" s="8"/>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B46" s="8"/>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B47" s="8"/>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B48" s="8"/>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B49" s="8"/>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B50" s="8"/>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51" s="8"/>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B52" s="8"/>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B53" s="8"/>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B54" s="8"/>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B55" s="8"/>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B56" s="8"/>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B57" s="8"/>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B58" s="8"/>
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B59" s="8"/>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B60" s="8"/>
+    </row>
+    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B61" s="8"/>
+    </row>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B62" s="8"/>
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B63" s="8"/>
+    </row>
+    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B64" s="8"/>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B65" s="8"/>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B66" s="8"/>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B67" s="8"/>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B68" s="8"/>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B69" s="8"/>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B70" s="8"/>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B71" s="8"/>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B72" s="8"/>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B73" s="8"/>
     </row>
     <row r="1048576" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1048576" s="6">
         <f>COUNT(C2:C1048575)</f>
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added set icons. Added set title component
Added a component which returns an SVG set icon with a colo representing a rarity of a card. Added a title element for a set including an it's icon
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7BA7186-EC4B-4370-AC7A-55B39B8C1BEE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EF3720D-EDF2-4FBA-803A-6BBEE118FC00}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2865" yWindow="825" windowWidth="21600" windowHeight="14460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -178,7 +178,7 @@
     <t>Debugging a problem with a very slow mouseMove-eventhandler attached to a window containing a table. For some reason it fires hundreds of invokeGuardedCallback-events. Concluded it should go away in a production build</t>
   </si>
   <si>
-    <t>Styled the card table nicely. The table now shows the card image when hovering the mouse over it and also works as a link to the card's own view</t>
+    <t>Styled the card table nicely. The table now shows the card image when hovering the mouse over it and also works as a link to the card's own view. It works ok in a prod build</t>
   </si>
 </sst>
 </file>
@@ -567,8 +567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -861,7 +861,7 @@
         <v>43</v>
       </c>
       <c r="C26" s="6">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="45" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added a single card info page
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EF3720D-EDF2-4FBA-803A-6BBEE118FC00}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C805C556-C08A-42AC-A7B2-8D879AF9FE36}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2865" yWindow="825" windowWidth="21600" windowHeight="14460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
   <si>
     <t>Task</t>
   </si>
@@ -179,6 +179,12 @@
   </si>
   <si>
     <t>Styled the card table nicely. The table now shows the card image when hovering the mouse over it and also works as a link to the card's own view. It works ok in a prod build</t>
+  </si>
+  <si>
+    <t>Added a component which returns an SVG set icon with a colo representing a rarity of a card. Added a title element for a set including an it's icon</t>
+  </si>
+  <si>
+    <t>Finished a decent version of a view for a single card info page</t>
   </si>
 </sst>
 </file>
@@ -568,7 +574,7 @@
   <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -875,11 +881,27 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="8"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B29" s="8"/>
+    <row r="28" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>43676</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>43677</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="6">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B30" s="8"/>
@@ -1016,7 +1038,7 @@
     <row r="1048576" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1048576" s="6">
         <f>COUNT(C2:C1048575)</f>
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Small refractos. Added functional Routes for a card view and a set view in the frontend and one small route for the backend
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C805C556-C08A-42AC-A7B2-8D879AF9FE36}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20AE32F4-4496-474F-9DB0-7C6A38C67A2E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2865" yWindow="825" windowWidth="21600" windowHeight="14460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
   <si>
     <t>Task</t>
   </si>
@@ -185,6 +185,9 @@
   </si>
   <si>
     <t>Finished a decent version of a view for a single card info page</t>
+  </si>
+  <si>
+    <t>Small refractos. Added functional Routes for a card view and a set view in the frontend and one small route for the backend</t>
   </si>
 </sst>
 </file>
@@ -573,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -903,8 +906,16 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B30" s="8"/>
+    <row r="30" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>43677</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C30" s="5">
+        <v>2.5</v>
+      </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B31" s="8"/>
@@ -1038,7 +1049,7 @@
     <row r="1048576" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1048576" s="6">
         <f>COUNT(C2:C1048575)</f>
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed manacost fonts not being imported properly. Fixed main site layout
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20AE32F4-4496-474F-9DB0-7C6A38C67A2E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC5412B4-9A69-4CB4-8621-AB62871C5D44}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2865" yWindow="825" windowWidth="21600" windowHeight="14460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
   <si>
     <t>Task</t>
   </si>
@@ -188,6 +188,9 @@
   </si>
   <si>
     <t>Small refractos. Added functional Routes for a card view and a set view in the frontend and one small route for the backend</t>
+  </si>
+  <si>
+    <t>Figuring out how to layout the main site container so that the footer is always pushed in the bottom and the &lt;main&gt; container takes up the space</t>
   </si>
 </sst>
 </file>
@@ -576,8 +579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -917,11 +920,20 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B31" s="8"/>
+    <row r="31" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>43677</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C31" s="6">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B32" s="8"/>
+      <c r="C32" s="5"/>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="8"/>
@@ -1049,7 +1061,7 @@
     <row r="1048576" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1048576" s="6">
         <f>COUNT(C2:C1048575)</f>
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a type icon component to display card types nicely
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC5412B4-9A69-4CB4-8621-AB62871C5D44}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A01AD92-3CA4-4309-A634-D609B76C3425}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2865" yWindow="825" windowWidth="21600" windowHeight="14460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -190,7 +190,7 @@
     <t>Small refractos. Added functional Routes for a card view and a set view in the frontend and one small route for the backend</t>
   </si>
   <si>
-    <t>Figuring out how to layout the main site container so that the footer is always pushed in the bottom and the &lt;main&gt; container takes up the space</t>
+    <t>Figuring out how to layout the main site container so that the footer is always pushed in the bottom and the &lt;main&gt; container takes up the space. Fixed manacost fonts not being imported properly.</t>
   </si>
 </sst>
 </file>
@@ -579,7 +579,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
@@ -920,7 +920,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>43677</v>
       </c>
@@ -928,7 +928,7 @@
         <v>48</v>
       </c>
       <c r="C31" s="6">
-        <v>1.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Small fixes. Working on the cardtable for building decks
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A01AD92-3CA4-4309-A634-D609B76C3425}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AE74C11-446A-47E8-8B03-A44134F4009B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2865" yWindow="825" windowWidth="21600" windowHeight="14460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
   <si>
     <t>Task</t>
   </si>
@@ -191,6 +191,15 @@
   </si>
   <si>
     <t>Figuring out how to layout the main site container so that the footer is always pushed in the bottom and the &lt;main&gt; container takes up the space. Fixed manacost fonts not being imported properly.</t>
+  </si>
+  <si>
+    <t>Added a type icon component to display card types nicely</t>
+  </si>
+  <si>
+    <t>04/08/2019 - 05/08/2019</t>
+  </si>
+  <si>
+    <t>Small fixes. Woking on a cardtable for editing decks, finished styling the basic table component</t>
   </si>
 </sst>
 </file>
@@ -266,9 +275,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -293,9 +301,16 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="4"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -579,489 +594,504 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="56.140625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="10" style="6" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="56.140625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="10" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="4">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>1.5</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="4">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="4">
         <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="4">
         <v>1.5</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="4">
         <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="4">
         <v>4.5</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="4">
         <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="4">
         <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
+      <c r="A18" s="12">
         <v>43664</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
+      <c r="A19" s="12">
         <v>43669</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="4">
         <v>1.5</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
+      <c r="A20" s="12">
         <v>43669</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20" s="5">
         <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
+      <c r="A21" s="12">
         <v>43670</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C21" s="5">
         <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
+      <c r="A22" s="12">
         <v>43670</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C22" s="5">
         <v>1.5</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
+      <c r="A23" s="12">
         <v>43671</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C23" s="5">
         <v>2.5</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
+      <c r="A24" s="12">
         <v>43671</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C24" s="5">
         <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
+      <c r="A25" s="12">
         <v>43672</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="6">
+      <c r="C25" s="5">
         <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A26" s="11" t="s">
+      <c r="A26" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="6">
+      <c r="C26" s="5">
         <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
+      <c r="A27" s="12">
         <v>43675</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="6">
+      <c r="C27" s="5">
         <v>5</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
+      <c r="A28" s="12">
         <v>43676</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C28" s="6">
+      <c r="C28" s="5">
         <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
+      <c r="A29" s="12">
         <v>43677</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="6">
+      <c r="C29" s="5">
         <v>1.5</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
+      <c r="A30" s="12">
         <v>43677</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C30" s="5">
+      <c r="C30" s="4">
         <v>2.5</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
+      <c r="A31" s="12">
         <v>43677</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C31" s="6">
+      <c r="C31" s="5">
         <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B32" s="8"/>
-      <c r="C32" s="5"/>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" s="8"/>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" s="8"/>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35" s="8"/>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B36" s="8"/>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B37" s="8"/>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B38" s="8"/>
-    </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B39" s="8"/>
-    </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B40" s="8"/>
-    </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B41" s="8"/>
-    </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B42" s="8"/>
-    </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B43" s="8"/>
-    </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B44" s="8"/>
-    </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B45" s="8"/>
-    </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B46" s="8"/>
-    </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B47" s="8"/>
-    </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B48" s="8"/>
+      <c r="A32" s="12">
+        <v>43679</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C32" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C33" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="7"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="7"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="7"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B37" s="7"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B38" s="7"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B39" s="7"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B40" s="7"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B41" s="7"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B42" s="7"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B43" s="7"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B44" s="7"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B45" s="7"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B46" s="7"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B47" s="7"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B48" s="7"/>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B49" s="8"/>
+      <c r="B49" s="7"/>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B50" s="8"/>
+      <c r="B50" s="7"/>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B51" s="8"/>
+      <c r="B51" s="7"/>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B52" s="8"/>
+      <c r="B52" s="7"/>
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B53" s="8"/>
+      <c r="B53" s="7"/>
     </row>
     <row r="54" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B54" s="8"/>
+      <c r="B54" s="7"/>
     </row>
     <row r="55" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B55" s="8"/>
+      <c r="B55" s="7"/>
     </row>
     <row r="56" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B56" s="8"/>
+      <c r="B56" s="7"/>
     </row>
     <row r="57" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B57" s="8"/>
+      <c r="B57" s="7"/>
     </row>
     <row r="58" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B58" s="8"/>
+      <c r="B58" s="7"/>
     </row>
     <row r="59" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B59" s="8"/>
+      <c r="B59" s="7"/>
     </row>
     <row r="60" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B60" s="8"/>
+      <c r="B60" s="7"/>
     </row>
     <row r="61" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B61" s="8"/>
+      <c r="B61" s="7"/>
     </row>
     <row r="62" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B62" s="8"/>
+      <c r="B62" s="7"/>
     </row>
     <row r="63" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B63" s="8"/>
+      <c r="B63" s="7"/>
     </row>
     <row r="64" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B64" s="8"/>
+      <c r="B64" s="7"/>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B65" s="8"/>
+      <c r="B65" s="7"/>
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B66" s="8"/>
+      <c r="B66" s="7"/>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B67" s="8"/>
+      <c r="B67" s="7"/>
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B68" s="8"/>
+      <c r="B68" s="7"/>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B69" s="8"/>
+      <c r="B69" s="7"/>
     </row>
     <row r="70" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B70" s="8"/>
+      <c r="B70" s="7"/>
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B71" s="8"/>
+      <c r="B71" s="7"/>
     </row>
     <row r="72" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B72" s="8"/>
+      <c r="B72" s="7"/>
     </row>
     <row r="73" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B73" s="8"/>
+      <c r="B73" s="7"/>
     </row>
     <row r="1048576" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C1048576" s="6">
+      <c r="C1048576" s="5">
         <f>COUNT(C2:C1048575)</f>
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Enabled fancy sorting for deckbuilder cardtable
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AE74C11-446A-47E8-8B03-A44134F4009B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5B0EB43-9B14-4376-B17E-5B4558877798}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2865" yWindow="825" windowWidth="21600" windowHeight="14460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
   <si>
     <t>Task</t>
   </si>
@@ -200,6 +200,12 @@
   </si>
   <si>
     <t>Small fixes. Woking on a cardtable for editing decks, finished styling the basic table component</t>
+  </si>
+  <si>
+    <t>05/08/2019 - 06/08/2019</t>
+  </si>
+  <si>
+    <t>The cardtable for deck editing can now be sorted nicely</t>
   </si>
 </sst>
 </file>
@@ -595,7 +601,7 @@
   <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -968,8 +974,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B34" s="7"/>
+    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C34" s="5">
+        <v>5</v>
+      </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B35" s="7"/>
@@ -1091,7 +1105,7 @@
     <row r="1048576" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1048576" s="5">
         <f>COUNT(C2:C1048575)</f>
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
The cards in the cardtable for deck editing can now be incremented and decremented. Added some useful functions in utils. Small fixes to sorting
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5B0EB43-9B14-4376-B17E-5B4558877798}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6521A4B6-5F84-49E9-87B5-C7513C1420CD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2865" yWindow="825" windowWidth="21600" windowHeight="14460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
   <si>
     <t>Task</t>
   </si>
@@ -206,6 +206,12 @@
   </si>
   <si>
     <t>The cardtable for deck editing can now be sorted nicely</t>
+  </si>
+  <si>
+    <t>The cards in the cardtable for deck editing can now be incremented and decremented. Added some useful functions in utils</t>
+  </si>
+  <si>
+    <t>Small fixes to sorting</t>
   </si>
 </sst>
 </file>
@@ -601,7 +607,7 @@
   <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -985,11 +991,27 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B35" s="7"/>
+    <row r="35" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35" s="11">
+        <v>43683</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C35" s="5">
+        <v>2.5</v>
+      </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B36" s="7"/>
+      <c r="A36" s="11">
+        <v>43683</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C36" s="5">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B37" s="7"/>
@@ -1105,7 +1127,7 @@
     <row r="1048576" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1048576" s="5">
         <f>COUNT(C2:C1048575)</f>
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Small fixes. Cards can now be transferred between two tables.
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6521A4B6-5F84-49E9-87B5-C7513C1420CD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A144DAE9-8D4D-445B-A32B-725E87F89EEA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2865" yWindow="825" windowWidth="21600" windowHeight="14460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="57">
   <si>
     <t>Task</t>
   </si>
@@ -212,6 +212,9 @@
   </si>
   <si>
     <t>Small fixes to sorting</t>
+  </si>
+  <si>
+    <t>The cards can now be transferred between two tables by doubleclick</t>
   </si>
 </sst>
 </file>
@@ -607,7 +610,7 @@
   <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1013,8 +1016,16 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B37" s="7"/>
+    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="11">
+        <v>43684</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C37" s="5">
+        <v>4</v>
+      </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B38" s="7"/>
@@ -1127,7 +1138,7 @@
     <row r="1048576" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1048576" s="5">
         <f>COUNT(C2:C1048575)</f>
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added mutliple different plots for various deck statistics
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A144DAE9-8D4D-445B-A32B-725E87F89EEA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7419141-DC96-4332-8961-CB572C4F7BBF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2865" yWindow="825" windowWidth="21600" windowHeight="14460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
   <si>
     <t>Task</t>
   </si>
@@ -215,6 +215,12 @@
   </si>
   <si>
     <t>The cards can now be transferred between two tables by doubleclick</t>
+  </si>
+  <si>
+    <t>Performance fixes, looking into plots of the deck's stats</t>
+  </si>
+  <si>
+    <t>Added mutliple different plots for various deck statistics</t>
   </si>
 </sst>
 </file>
@@ -610,7 +616,7 @@
   <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1028,10 +1034,26 @@
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B38" s="7"/>
+      <c r="A38" s="11">
+        <v>43684</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C38" s="5">
+        <v>2</v>
+      </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B39" s="7"/>
+      <c r="A39" s="11">
+        <v>43685</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C39" s="5">
+        <v>5</v>
+      </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B40" s="7"/>
@@ -1138,7 +1160,7 @@
     <row r="1048576" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1048576" s="5">
         <f>COUNT(C2:C1048575)</f>
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added pickers for basic lands for a deck. Adjusted the plots
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7419141-DC96-4332-8961-CB572C4F7BBF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80B90D35-60E2-4DC8-8591-AC0874C4F12A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2865" yWindow="825" windowWidth="21600" windowHeight="14460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="60">
   <si>
     <t>Task</t>
   </si>
@@ -221,6 +221,9 @@
   </si>
   <si>
     <t>Added mutliple different plots for various deck statistics</t>
+  </si>
+  <si>
+    <t>Added pickers for basic lands for a deck. Adjusted the plots</t>
   </si>
 </sst>
 </file>
@@ -616,7 +619,7 @@
   <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1056,7 +1059,15 @@
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B40" s="7"/>
+      <c r="A40" s="11">
+        <v>43689</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C40" s="5">
+        <v>2</v>
+      </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B41" s="7"/>
@@ -1160,7 +1171,7 @@
     <row r="1048576" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1048576" s="5">
         <f>COUNT(C2:C1048575)</f>
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working in deck view. Added titles to plots
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80B90D35-60E2-4DC8-8591-AC0874C4F12A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72827312-07C6-4C7D-B616-6A8B3569B9D9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2865" yWindow="825" windowWidth="21600" windowHeight="14460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
   <si>
     <t>Task</t>
   </si>
@@ -224,6 +224,9 @@
   </si>
   <si>
     <t>Added pickers for basic lands for a deck. Adjusted the plots</t>
+  </si>
+  <si>
+    <t>Added a simple deck view. Added titles to plots</t>
   </si>
 </sst>
 </file>
@@ -619,7 +622,7 @@
   <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1070,7 +1073,15 @@
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B41" s="7"/>
+      <c r="A41" s="11">
+        <v>43689</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C41" s="5">
+        <v>3</v>
+      </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B42" s="7"/>
@@ -1171,7 +1182,7 @@
     <row r="1048576" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1048576" s="5">
         <f>COUNT(C2:C1048575)</f>
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished a decent deck view. Working on deck edit card tables
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72827312-07C6-4C7D-B616-6A8B3569B9D9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C71E0A9-EF39-4D4C-9561-8F64B49E3416}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2865" yWindow="825" windowWidth="21600" windowHeight="14460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
   <si>
     <t>Task</t>
   </si>
@@ -227,6 +227,9 @@
   </si>
   <si>
     <t>Added a simple deck view. Added titles to plots</t>
+  </si>
+  <si>
+    <t>Finished a decent deck view. Working on deck edit card tables</t>
   </si>
 </sst>
 </file>
@@ -622,7 +625,7 @@
   <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1083,8 +1086,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B42" s="7"/>
+    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="11">
+        <v>43690</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C42" s="5">
+        <v>5</v>
+      </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B43" s="7"/>
@@ -1182,7 +1193,7 @@
     <row r="1048576" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1048576" s="5">
         <f>COUNT(C2:C1048575)</f>
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
The deckbuilder card table now has decent controls for selecting/transferring cards
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C71E0A9-EF39-4D4C-9561-8F64B49E3416}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0259E9D0-33C7-452F-874F-EFAA63B821E4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2865" yWindow="825" windowWidth="21600" windowHeight="14460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
   <si>
     <t>Task</t>
   </si>
@@ -230,6 +230,12 @@
   </si>
   <si>
     <t>Finished a decent deck view. Working on deck edit card tables</t>
+  </si>
+  <si>
+    <t>14/08/2019-15/08/2019</t>
+  </si>
+  <si>
+    <t>The deckbuilder card table now has decent controls for selecting/transferring cards. Tested some static builds for Storybook</t>
   </si>
 </sst>
 </file>
@@ -625,7 +631,7 @@
   <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1097,8 +1103,16 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B43" s="7"/>
+    <row r="43" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C43" s="5">
+        <v>6</v>
+      </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B44" s="7"/>
@@ -1193,7 +1207,7 @@
     <row r="1048576" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1048576" s="5">
         <f>COUNT(C2:C1048575)</f>
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added User and Deck tables with appropriate connections in the backend database. Added simple support for user registration with flask-wtf forms
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0259E9D0-33C7-452F-874F-EFAA63B821E4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDA95193-76ED-400D-B598-5A981A652D9D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2865" yWindow="825" windowWidth="21600" windowHeight="14460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="66">
   <si>
     <t>Task</t>
   </si>
@@ -236,6 +236,12 @@
   </si>
   <si>
     <t>The deckbuilder card table now has decent controls for selecting/transferring cards. Tested some static builds for Storybook</t>
+  </si>
+  <si>
+    <t>16/08/2019-19/08/2019</t>
+  </si>
+  <si>
+    <t>Added User and Deck tables with appropriate connections in the backend database. Added simple support for user registration with flask-wtf forms</t>
   </si>
 </sst>
 </file>
@@ -631,7 +637,7 @@
   <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1114,8 +1120,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B44" s="7"/>
+    <row r="44" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C44" s="5">
+        <v>8</v>
+      </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B45" s="7"/>
@@ -1207,7 +1221,7 @@
     <row r="1048576" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1048576" s="5">
         <f>COUNT(C2:C1048575)</f>
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added JWT authentication to the backend along with routes for Login, Logout, Signup and token verification
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDA95193-76ED-400D-B598-5A981A652D9D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F45B412-77E2-418E-A7A7-33A8D875C93E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2865" yWindow="825" windowWidth="21600" windowHeight="14460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="68">
   <si>
     <t>Task</t>
   </si>
@@ -242,6 +242,12 @@
   </si>
   <si>
     <t>Added User and Deck tables with appropriate connections in the backend database. Added simple support for user registration with flask-wtf forms</t>
+  </si>
+  <si>
+    <t>Reading about JWT authentication methods</t>
+  </si>
+  <si>
+    <t>Added JWT authentication to the backend along with routes for Login, Logout, Signup and token verification</t>
   </si>
 </sst>
 </file>
@@ -636,8 +642,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1132,10 +1138,26 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B45" s="7"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B46" s="7"/>
+      <c r="A45" s="11">
+        <v>43696</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C45" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="11">
+        <v>43697</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C46" s="5">
+        <v>3.5</v>
+      </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B47" s="7"/>
@@ -1221,7 +1243,7 @@
     <row r="1048576" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1048576" s="5">
         <f>COUNT(C2:C1048575)</f>
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added basic login and signup views for the frontend
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F45B412-77E2-418E-A7A7-33A8D875C93E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44F1C81-42E2-41A4-A4F3-6016AC23C71D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2865" yWindow="825" windowWidth="21600" windowHeight="14460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="70">
   <si>
     <t>Task</t>
   </si>
@@ -248,6 +248,12 @@
   </si>
   <si>
     <t>Added JWT authentication to the backend along with routes for Login, Logout, Signup and token verification</t>
+  </si>
+  <si>
+    <t>20/08/2019-21/08/2019</t>
+  </si>
+  <si>
+    <t>Added basic login and signup views for the frontend</t>
   </si>
 </sst>
 </file>
@@ -643,7 +649,7 @@
   <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1159,8 +1165,16 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B47" s="7"/>
+    <row r="47" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C47" s="5">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B48" s="7"/>
@@ -1243,7 +1257,7 @@
     <row r="1048576" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1048576" s="5">
         <f>COUNT(C2:C1048575)</f>
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added auth services and login flow
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44F1C81-42E2-41A4-A4F3-6016AC23C71D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E66E8AE2-DB66-4260-AB28-FFF9B0F8FD61}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2865" yWindow="825" windowWidth="21600" windowHeight="14460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="71">
   <si>
     <t>Task</t>
   </si>
@@ -254,6 +254,9 @@
   </si>
   <si>
     <t>Added basic login and signup views for the frontend</t>
+  </si>
+  <si>
+    <t>Added auth services and login flow</t>
   </si>
 </sst>
 </file>
@@ -649,7 +652,7 @@
   <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1177,7 +1180,15 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B48" s="7"/>
+      <c r="A48" s="11">
+        <v>43698</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C48" s="5">
+        <v>2</v>
+      </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" s="7"/>
@@ -1257,7 +1268,7 @@
     <row r="1048576" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1048576" s="5">
         <f>COUNT(C2:C1048575)</f>
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added authorized routes for creating, getting, deleting and editing decks. Decks now have many to many relationships to cards both for the maindeck and sideboard
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFE26DD4-F63A-4BF0-BCED-BEB73C5F3341}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7E397A7-17FF-49ED-A3B9-3C0BE12C92D1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2865" yWindow="825" windowWidth="21600" windowHeight="14460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="74">
   <si>
     <t>Task</t>
   </si>
@@ -257,6 +257,15 @@
   </si>
   <si>
     <t>Added auth services and login flow</t>
+  </si>
+  <si>
+    <t>Added signup flow and small fixes</t>
+  </si>
+  <si>
+    <t>22/08/2019-23/08/2019</t>
+  </si>
+  <si>
+    <t>Added authorized routes for creating, getting, deleting and editing decks. Decks now have many to many relationships to cards both for the maindeck and sideboard</t>
   </si>
 </sst>
 </file>
@@ -652,7 +661,7 @@
   <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1190,52 +1199,68 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B49" s="7"/>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B50" s="7"/>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="11">
+        <v>43699</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C49" s="5">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C50" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B51" s="7"/>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B52" s="7"/>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B53" s="7"/>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B54" s="7"/>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B55" s="7"/>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B56" s="7"/>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B57" s="7"/>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B58" s="7"/>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B59" s="7"/>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B60" s="7"/>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B61" s="7"/>
     </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B62" s="7"/>
     </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B63" s="7"/>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B64" s="7"/>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.25">
@@ -1268,7 +1293,7 @@
     <row r="1048576" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1048576" s="5">
         <f>COUNT(C2:C1048575)</f>
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Small fixes and added a view for creating sealed decks
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7E397A7-17FF-49ED-A3B9-3C0BE12C92D1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F69CE3D2-1E2C-46BB-BA42-EC77566B3FE6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2865" yWindow="825" windowWidth="21600" windowHeight="14460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="76">
   <si>
     <t>Task</t>
   </si>
@@ -266,6 +266,12 @@
   </si>
   <si>
     <t>Added authorized routes for creating, getting, deleting and editing decks. Decks now have many to many relationships to cards both for the maindeck and sideboard</t>
+  </si>
+  <si>
+    <t>26/08/2019-29/08/2019</t>
+  </si>
+  <si>
+    <t>Small fixes and added a view for creating sealed decks</t>
   </si>
 </sst>
 </file>
@@ -661,7 +667,7 @@
   <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1221,8 +1227,16 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B51" s="7"/>
+    <row r="51" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C51" s="5">
+        <v>14</v>
+      </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B52" s="7"/>
@@ -1293,7 +1307,7 @@
     <row r="1048576" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1048576" s="5">
         <f>COUNT(C2:C1048575)</f>
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
general fixes, refractorings and performance improvements for the frontend
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C81AA31D-6121-4B0F-AD42-703CE70C9F46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A24E5D9-DD60-4D67-A969-1469367E3B17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="14460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="79">
   <si>
     <t>Task</t>
   </si>
@@ -288,6 +288,10 @@
 - Added hooks for editing/creating decks and accommodated the backend to handle the requests
 - Creating/editing decks flow now works well, still missing adding basic lands
 </t>
+  </si>
+  <si>
+    <t>Added good alerts for editing/creating decks.
+Figuring out how to use PostgreSQL</t>
   </si>
 </sst>
 </file>
@@ -683,7 +687,7 @@
   <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1265,8 +1269,16 @@
         <v>24</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B53" s="7"/>
+    <row r="53" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="11">
+        <v>43901</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C53" s="5">
+        <v>5</v>
+      </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B54" s="7"/>
@@ -1331,7 +1343,7 @@
     <row r="1048576" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1048576" s="5">
         <f>COUNT(C2:C1048575)</f>
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed time and readme
</commit_message>
<xml_diff>
--- a/Time.xlsx
+++ b/Time.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB79C717-50B0-494C-8B10-75E5E90FFC68}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31708DD0-8500-4FBA-ABCE-A90ECAFA07F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2700" yWindow="75" windowWidth="21600" windowHeight="14715" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="83">
   <si>
     <t>Task</t>
   </si>
@@ -277,30 +277,39 @@
   </si>
   <si>
     <t>1/9/2019-11/03/2020</t>
+  </si>
+  <si>
+    <t>Added good alerts for editing/creating decks.
+Figuring out how to use PostgreSQL</t>
+  </si>
+  <si>
+    <t>- Added a PostgreSQL database to Heroku and figured out how to transfer the local database there. Now backend is using the Heroku database in the cloud
+- Did a lot of general fixes, refractorings and performance improvements for the card list components</t>
+  </si>
+  <si>
+    <t>- Finally got the database working after debugging for a long time
+- General fixes and refractorings
+- Added routes for users to view their own created decks</t>
+  </si>
+  <si>
+    <t>Total Hours:</t>
+  </si>
+  <si>
+    <t>- Deployed also the frontend to Heroku
+- Added a home page
+- Wrote a more accurate description of the project and what it contains
+-Added some last minute refractorings and fixes</t>
   </si>
   <si>
     <t xml:space="preserve">This work was mostly done during the weeks 9-11. I did some smaller things before but didn’t really want to commit them. I estimate that this took about 3-4 full 8-hour days of work 
 - Reading/testing on making Flask/React work together. Looks like the best way is to keep them completely separate
 - A lot of refractoring and fixes for various errors
 - Made private routes work as intended
-- Performance fixes with memoizing components because of long lists of 
+- Performance fixes with memoizing components because of long lists of cards
 - Put the created views together in the routing
 - Added hooks for editing/creating decks and accommodated the backend to handle the requests
 - Creating/editing decks flow now works well, still missing adding basic lands
 </t>
-  </si>
-  <si>
-    <t>Added good alerts for editing/creating decks.
-Figuring out how to use PostgreSQL</t>
-  </si>
-  <si>
-    <t>- Added a PostgreSQL database to Heroku and figured out how to transfer the local database there. Now backend is using the Heroku database in the cloud
-- Did a lot of general fixes, refractorings and performance improvements for the card list components</t>
-  </si>
-  <si>
-    <t>- Finally got the database working after debugging for a long time
-- General fixes and refractorings
-- Added routes for users to view their own created decks</t>
   </si>
 </sst>
 </file>
@@ -696,7 +705,7 @@
   <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1272,7 +1281,7 @@
         <v>76</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="C52" s="5">
         <v>24</v>
@@ -1283,7 +1292,7 @@
         <v>43901</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C53" s="5">
         <v>5</v>
@@ -1294,7 +1303,7 @@
         <v>43902</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C54" s="5">
         <v>6</v>
@@ -1305,17 +1314,31 @@
         <v>43903</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C55" s="5">
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B56" s="7"/>
+    <row r="56" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A56" s="11">
+        <v>43904</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C56" s="5">
+        <v>7</v>
+      </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B57" s="7"/>
+      <c r="B57" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C57" s="4">
+        <f>SUM(C2:C56)</f>
+        <v>234</v>
+      </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B58" s="7"/>
@@ -1368,7 +1391,7 @@
     <row r="1048576" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C1048576" s="5">
         <f>COUNT(C2:C1048575)</f>
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>